<commit_message>
clean up and get session outputs
</commit_message>
<xml_diff>
--- a/data/2021MND/MND_teams_2021.xlsx
+++ b/data/2021MND/MND_teams_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rescorp.sharepoint.com/sites/W-Drive/Shared Documents/KHuynh Files/dimensions_api_publication_data_pull/update_runs/outputs/MND_outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{75E65C17-26F1-7440-B2B9-F745B1CED7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8036857F-D69C-6542-B0B7-2DC9D5E0F28B}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{75E65C17-26F1-7440-B2B9-F745B1CED7E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15317DC3-2D31-48BD-A09A-6D1C62434743}"/>
   <bookViews>
     <workbookView xWindow="-34940" yWindow="840" windowWidth="27640" windowHeight="16940" xr2:uid="{BBC96F5E-EEBA-3447-9142-7F92B572A6FD}"/>
   </bookViews>
@@ -760,7 +760,7 @@
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="128.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60" customWidth="1"/>
     <col min="6" max="6" width="44.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1270,6 +1270,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007224E5F0053A78439374553BFE681CBE" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b5eb0d01675599322aaa2854ad7b42fa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d36ef3fb-7dd2-43d9-a7cf-5a13da02748c" xmlns:ns3="c9d5ca3a-33f2-45cf-9ce6-efa5cf7cd8ed" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="badfa3da0024526f3837a4caf6734a32" ns2:_="" ns3:_="">
     <xsd:import namespace="d36ef3fb-7dd2-43d9-a7cf-5a13da02748c"/>
@@ -1524,19 +1533,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C175319-EE33-42E6-950C-09C836B60A6E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A20631F-CB7A-4C38-8C4F-F4E2DC93C107}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A20631F-CB7A-4C38-8C4F-F4E2DC93C107}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C175319-EE33-42E6-950C-09C836B60A6E}"/>
 </file>
</xml_diff>